<commit_message>
from updated data extraction scripts
</commit_message>
<xml_diff>
--- a/DataCreated/BQESEdatTW_WFD2016.xlsx
+++ b/DataCreated/BQESEdatTW_WFD2016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uapt33090-my.sharepoint.com/personal/heliana_teixeira_ua_pt/Documents/Rdir/WFD-TRaC-data-upto2022/DataCreated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helianateixeira/Documents/Rdir/WFD-TRaC-data-upto2022/DataCreated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_03C8D48CE2EF947B63753E780C2113E69870FD4A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9E895E6-93C8-0746-8A95-B34155D341C6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEB9DD7-2332-104C-A996-498663315A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="44180" windowHeight="22000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7120" yWindow="2440" windowWidth="19980" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1336,10 +1336,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AL112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3138,7 +3139,7 @@
         <v>14.25</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -3297,7 +3298,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -3341,7 +3342,7 @@
         <v>124.5</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -3737,7 +3738,7 @@
         <v>5.3046666666666704</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -3775,7 +3776,7 @@
         <v>33.872916666666697</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -4141,7 +4142,7 @@
         <v>27.274999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>145</v>
       </c>
@@ -4191,7 +4192,7 @@
         <v>0.77814090909090905</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>151</v>
       </c>
@@ -4241,7 +4242,7 @@
         <v>0.51623564393939403</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>153</v>
       </c>
@@ -4291,7 +4292,7 @@
         <v>0.32261944444444401</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>155</v>
       </c>
@@ -4347,7 +4348,7 @@
         <v>0.98553571428571396</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>157</v>
       </c>
@@ -4388,7 +4389,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>159</v>
       </c>
@@ -4512,7 +4513,7 @@
         <v>4.3262499999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>166</v>
       </c>
@@ -4562,7 +4563,7 @@
         <v>0.34977916666666697</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>169</v>
       </c>
@@ -4609,7 +4610,7 @@
         <v>0.51188636363636397</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -4665,7 +4666,7 @@
         <v>1.1571428571428599</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>173</v>
       </c>
@@ -4715,7 +4716,7 @@
         <v>0.83622361111111099</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -4774,7 +4775,7 @@
         <v>3.9203653005573198</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>178</v>
       </c>
@@ -4895,7 +4896,7 @@
         <v>1.0645833333333301</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>183</v>
       </c>
@@ -4954,7 +4955,7 @@
         <v>3.68057304398998</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>185</v>
       </c>
@@ -5004,7 +5005,7 @@
         <v>0.85188194444444398</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>187</v>
       </c>
@@ -5054,7 +5055,7 @@
         <v>0.33703181818181799</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>189</v>
       </c>
@@ -5113,7 +5114,7 @@
         <v>3.36084875734623</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>192</v>
       </c>
@@ -5172,7 +5173,7 @@
         <v>4.3266784383425199</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>195</v>
       </c>
@@ -5231,7 +5232,7 @@
         <v>3.3675076165606299</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>198</v>
       </c>
@@ -5290,7 +5291,7 @@
         <v>2.8550274509946898</v>
       </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>200</v>
       </c>
@@ -5349,7 +5350,7 @@
         <v>3.8125356507156098</v>
       </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>202</v>
       </c>
@@ -5396,7 +5397,7 @@
         <v>1.9749298611111099</v>
       </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>204</v>
       </c>
@@ -5443,7 +5444,7 @@
         <v>0.37463999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>206</v>
       </c>
@@ -5502,7 +5503,7 @@
         <v>3.0086461570794598</v>
       </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>208</v>
       </c>
@@ -5552,7 +5553,7 @@
         <v>0.481494166666667</v>
       </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>210</v>
       </c>
@@ -5608,7 +5609,7 @@
         <v>0.80535714285714299</v>
       </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>213</v>
       </c>
@@ -5729,7 +5730,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>217</v>
       </c>
@@ -5776,7 +5777,7 @@
         <v>0.34380333333333302</v>
       </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>219</v>
       </c>
@@ -5826,7 +5827,7 @@
         <v>1.3314430555555601</v>
       </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>221</v>
       </c>
@@ -5876,7 +5877,7 @@
         <v>0.37785833333333302</v>
       </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>223</v>
       </c>
@@ -5923,7 +5924,7 @@
         <v>1.8364145833333301</v>
       </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>225</v>
       </c>
@@ -5982,7 +5983,7 @@
         <v>3.0024061410216198</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>227</v>
       </c>
@@ -6038,7 +6039,7 @@
         <v>1.2202380952381</v>
       </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>229</v>
       </c>
@@ -6171,7 +6172,7 @@
         <v>3.8308333333333302E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>235</v>
       </c>
@@ -6271,7 +6272,7 @@
         <v>2.72833333333333E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>241</v>
       </c>
@@ -6389,7 +6390,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>246</v>
       </c>
@@ -6445,7 +6446,7 @@
         <v>1.28571428571429</v>
       </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>248</v>
       </c>
@@ -6974,7 +6975,7 @@
         <v>0.43888888888888899</v>
       </c>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>267</v>
       </c>
@@ -7042,7 +7043,7 @@
         <v>1.5021111111111101</v>
       </c>
     </row>
-    <row r="96" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>271</v>
       </c>
@@ -7618,7 +7619,7 @@
         <v>1.07937062937063E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>292</v>
       </c>
@@ -7686,7 +7687,7 @@
         <v>1.8473333333333299</v>
       </c>
     </row>
-    <row r="106" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>295</v>
       </c>
@@ -7724,7 +7725,7 @@
         <v>11.7092594089161</v>
       </c>
     </row>
-    <row r="107" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>299</v>
       </c>
@@ -8151,6 +8152,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AL112" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="23">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
update files synch with pc
</commit_message>
<xml_diff>
--- a/DataCreated/BQESEdatTW_WFD2016.xlsx
+++ b/DataCreated/BQESEdatTW_WFD2016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helianateixeira/Documents/Rdir/WFD-TRaC-data-upto2022/DataCreated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uapt33090-my.sharepoint.com/personal/heliana_teixeira_ua_pt/Documents/Rdir/WFD-TRaC-data-upto2022/DataCreated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEB9DD7-2332-104C-A996-498663315A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_03C8D48CE2EF947B63753E780C2113E69870FD4A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9E895E6-93C8-0746-8A95-B34155D341C6}"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="2440" windowWidth="19980" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="44180" windowHeight="22000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1336,11 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AL112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3139,7 +3138,7 @@
         <v>14.25</v>
       </c>
     </row>
-    <row r="28" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -3298,7 +3297,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="31" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -3342,7 +3341,7 @@
         <v>124.5</v>
       </c>
     </row>
-    <row r="32" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -3738,7 +3737,7 @@
         <v>5.3046666666666704</v>
       </c>
     </row>
-    <row r="38" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -3776,7 +3775,7 @@
         <v>33.872916666666697</v>
       </c>
     </row>
-    <row r="39" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -4142,7 +4141,7 @@
         <v>27.274999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>145</v>
       </c>
@@ -4192,7 +4191,7 @@
         <v>0.77814090909090905</v>
       </c>
     </row>
-    <row r="46" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>151</v>
       </c>
@@ -4242,7 +4241,7 @@
         <v>0.51623564393939403</v>
       </c>
     </row>
-    <row r="47" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>153</v>
       </c>
@@ -4292,7 +4291,7 @@
         <v>0.32261944444444401</v>
       </c>
     </row>
-    <row r="48" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>155</v>
       </c>
@@ -4348,7 +4347,7 @@
         <v>0.98553571428571396</v>
       </c>
     </row>
-    <row r="49" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>157</v>
       </c>
@@ -4389,7 +4388,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>159</v>
       </c>
@@ -4513,7 +4512,7 @@
         <v>4.3262499999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>166</v>
       </c>
@@ -4563,7 +4562,7 @@
         <v>0.34977916666666697</v>
       </c>
     </row>
-    <row r="53" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>169</v>
       </c>
@@ -4610,7 +4609,7 @@
         <v>0.51188636363636397</v>
       </c>
     </row>
-    <row r="54" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>1.1571428571428599</v>
       </c>
     </row>
-    <row r="55" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>173</v>
       </c>
@@ -4716,7 +4715,7 @@
         <v>0.83622361111111099</v>
       </c>
     </row>
-    <row r="56" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -4775,7 +4774,7 @@
         <v>3.9203653005573198</v>
       </c>
     </row>
-    <row r="57" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>178</v>
       </c>
@@ -4896,7 +4895,7 @@
         <v>1.0645833333333301</v>
       </c>
     </row>
-    <row r="59" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>183</v>
       </c>
@@ -4955,7 +4954,7 @@
         <v>3.68057304398998</v>
       </c>
     </row>
-    <row r="60" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>185</v>
       </c>
@@ -5005,7 +5004,7 @@
         <v>0.85188194444444398</v>
       </c>
     </row>
-    <row r="61" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>187</v>
       </c>
@@ -5055,7 +5054,7 @@
         <v>0.33703181818181799</v>
       </c>
     </row>
-    <row r="62" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>189</v>
       </c>
@@ -5114,7 +5113,7 @@
         <v>3.36084875734623</v>
       </c>
     </row>
-    <row r="63" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>192</v>
       </c>
@@ -5173,7 +5172,7 @@
         <v>4.3266784383425199</v>
       </c>
     </row>
-    <row r="64" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>195</v>
       </c>
@@ -5232,7 +5231,7 @@
         <v>3.3675076165606299</v>
       </c>
     </row>
-    <row r="65" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>198</v>
       </c>
@@ -5291,7 +5290,7 @@
         <v>2.8550274509946898</v>
       </c>
     </row>
-    <row r="66" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>200</v>
       </c>
@@ -5350,7 +5349,7 @@
         <v>3.8125356507156098</v>
       </c>
     </row>
-    <row r="67" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>202</v>
       </c>
@@ -5397,7 +5396,7 @@
         <v>1.9749298611111099</v>
       </c>
     </row>
-    <row r="68" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>204</v>
       </c>
@@ -5444,7 +5443,7 @@
         <v>0.37463999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>206</v>
       </c>
@@ -5503,7 +5502,7 @@
         <v>3.0086461570794598</v>
       </c>
     </row>
-    <row r="70" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>208</v>
       </c>
@@ -5553,7 +5552,7 @@
         <v>0.481494166666667</v>
       </c>
     </row>
-    <row r="71" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>210</v>
       </c>
@@ -5609,7 +5608,7 @@
         <v>0.80535714285714299</v>
       </c>
     </row>
-    <row r="72" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>213</v>
       </c>
@@ -5730,7 +5729,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="74" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>217</v>
       </c>
@@ -5777,7 +5776,7 @@
         <v>0.34380333333333302</v>
       </c>
     </row>
-    <row r="75" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>219</v>
       </c>
@@ -5827,7 +5826,7 @@
         <v>1.3314430555555601</v>
       </c>
     </row>
-    <row r="76" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>221</v>
       </c>
@@ -5877,7 +5876,7 @@
         <v>0.37785833333333302</v>
       </c>
     </row>
-    <row r="77" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>223</v>
       </c>
@@ -5924,7 +5923,7 @@
         <v>1.8364145833333301</v>
       </c>
     </row>
-    <row r="78" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>225</v>
       </c>
@@ -5983,7 +5982,7 @@
         <v>3.0024061410216198</v>
       </c>
     </row>
-    <row r="79" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>227</v>
       </c>
@@ -6039,7 +6038,7 @@
         <v>1.2202380952381</v>
       </c>
     </row>
-    <row r="80" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>229</v>
       </c>
@@ -6172,7 +6171,7 @@
         <v>3.8308333333333302E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>235</v>
       </c>
@@ -6272,7 +6271,7 @@
         <v>2.72833333333333E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>241</v>
       </c>
@@ -6390,7 +6389,7 @@
         <v>2.3333333333333299</v>
       </c>
     </row>
-    <row r="86" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>246</v>
       </c>
@@ -6446,7 +6445,7 @@
         <v>1.28571428571429</v>
       </c>
     </row>
-    <row r="87" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>248</v>
       </c>
@@ -6975,7 +6974,7 @@
         <v>0.43888888888888899</v>
       </c>
     </row>
-    <row r="95" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>267</v>
       </c>
@@ -7043,7 +7042,7 @@
         <v>1.5021111111111101</v>
       </c>
     </row>
-    <row r="96" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>271</v>
       </c>
@@ -7619,7 +7618,7 @@
         <v>1.07937062937063E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>292</v>
       </c>
@@ -7687,7 +7686,7 @@
         <v>1.8473333333333299</v>
       </c>
     </row>
-    <row r="106" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>295</v>
       </c>
@@ -7725,7 +7724,7 @@
         <v>11.7092594089161</v>
       </c>
     </row>
-    <row r="107" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>299</v>
       </c>
@@ -8152,13 +8151,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL112" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="23">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>